<commit_message>
Change model to Employee and add data
</commit_message>
<xml_diff>
--- a/Excel/ReportClosedXML3Format.xlsx
+++ b/Excel/ReportClosedXML3Format.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Customer Records" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Employee Records" sheetId="1" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -25,10 +25,25 @@
     <x:t>Address</x:t>
   </x:si>
   <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Salary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Birthday</x:t>
+  </x:si>
+  <x:si>
     <x:t>Andres</x:t>
   </x:si>
   <x:si>
     <x:t>Carrera 22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>andres@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-12-12</x:t>
   </x:si>
   <x:si>
     <x:t>Ana</x:t>
@@ -140,12 +155,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
-  <x:autoFilter ref="A1:C10"/>
-  <x:tableColumns count="3">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0">
+  <x:autoFilter ref="A1:F10"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="Name"/>
     <x:tableColumn id="2" name="Age"/>
     <x:tableColumn id="3" name="Address"/>
+    <x:tableColumn id="4" name="Email"/>
+    <x:tableColumn id="5" name="Salary"/>
+    <x:tableColumn id="6" name="Birthday"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -439,13 +457,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C10"/>
+  <x:dimension ref="A1:F10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -455,104 +473,194 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0">
         <x:v>18</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B3" s="0">
         <x:v>19</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E3" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="0">
         <x:v>25</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B5" s="0">
         <x:v>34</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E5" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B6" s="0">
         <x:v>65</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E6" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B7" s="0">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E7" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B8" s="0">
         <x:v>87</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E8" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B9" s="0">
         <x:v>56</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E9" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
       <x:c r="A10" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B10" s="0">
         <x:v>46</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="0">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add format to report
</commit_message>
<xml_diff>
--- a/Excel/ReportClosedXML3Format.xlsx
+++ b/Excel/ReportClosedXML3Format.xlsx
@@ -101,7 +101,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="5">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -109,13 +109,46 @@
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFF0000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FFB2BEB5"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FFFFFFFF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF000000"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -137,13 +170,41 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -462,98 +523,102 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <x:col min="2" max="4" width="9.140625" style="2" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:6">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
+      <x:c r="B1" s="4" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="C1" s="4" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+      <x:c r="D1" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="E1" s="4" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
+      <x:c r="F1" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
-      <x:c r="A2" s="0" t="s">
+    <x:row r="2" spans="1:6" s="3" customFormat="1">
+      <x:c r="A2" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B2" s="0">
+      <x:c r="B2" s="3">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="C2" s="3" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E2" s="0">
-        <x:v>1500000</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="D2" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="3">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F2" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" s="3" customFormat="1">
+      <x:c r="A3" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B3" s="0">
+      <x:c r="B3" s="3">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="C3" s="3" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E3" s="0">
-        <x:v>1500000</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="D3" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E3" s="3">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F3" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" s="3" customFormat="1">
+      <x:c r="A4" s="3" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B4" s="0">
+      <x:c r="B4" s="3">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="C4" s="3" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E4" s="0">
-        <x:v>1500000</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="D4" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="3">
+        <x:v>1500000</x:v>
+      </x:c>
+      <x:c r="F4" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
-      <x:c r="A5" s="0" t="s">
+      <x:c r="A5" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B5" s="0">
+      <x:c r="B5" s="2">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="C5" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
+      <x:c r="D5" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E5" s="0">
@@ -564,16 +629,16 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
-      <x:c r="A6" s="0" t="s">
+      <x:c r="A6" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B6" s="0">
+      <x:c r="B6" s="2">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="C6" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="D6" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E6" s="0">
@@ -584,16 +649,16 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
-      <x:c r="A7" s="0" t="s">
+      <x:c r="A7" s="1" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B7" s="0">
+      <x:c r="B7" s="2">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="C7" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="D7" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E7" s="0">
@@ -604,16 +669,16 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
-      <x:c r="A8" s="0" t="s">
+      <x:c r="A8" s="1" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B8" s="0">
+      <x:c r="B8" s="2">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
+      <x:c r="C8" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
+      <x:c r="D8" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E8" s="0">
@@ -624,16 +689,16 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
-      <x:c r="A9" s="0" t="s">
+      <x:c r="A9" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B9" s="0">
+      <x:c r="B9" s="2">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
+      <x:c r="C9" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
+      <x:c r="D9" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E9" s="0">
@@ -644,16 +709,16 @@
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
-      <x:c r="A10" s="0" t="s">
+      <x:c r="A10" s="1" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B10" s="0">
+      <x:c r="B10" s="2">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="C10" s="0" t="s">
+      <x:c r="C10" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s">
+      <x:c r="D10" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="E10" s="0">

</xml_diff>